<commit_message>
version 10/04 || import data from excel to db
</commit_message>
<xml_diff>
--- a/web/file.xlsx
+++ b/web/file.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Simple" sheetId="1" r:id="rId4"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
@@ -15,20 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
-  <si>
-    <t>Hello</t>
-  </si>
-  <si>
-    <t>world!</t>
-  </si>
-  <si>
-    <t>Miscellaneous glyphs</t>
-  </si>
-  <si>
-    <t>éàèùâêîôûëïüÿäöüç</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -365,41 +352,14 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>